<commit_message>
updated with class timing
</commit_message>
<xml_diff>
--- a/docs/Neha CS Waiver Learning Plan.xlsx
+++ b/docs/Neha CS Waiver Learning Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Start Date</t>
   </si>
@@ -73,14 +73,25 @@
   </si>
   <si>
     <t xml:space="preserve">Q&amp;A Review before the Interview &amp; get ready to present </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Class to review the work every Sunday @10AM </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -129,11 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,8 +674,14 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>